<commit_message>
Lectures and project name change
</commit_message>
<xml_diff>
--- a/LectureSpring2019.xlsx
+++ b/LectureSpring2019.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Fatih/GitHub/dataism/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF0D57C6-A77F-324C-BFDB-03E25423D46C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE0A6241-9352-4F45-B29F-2DDD247981DF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20" yWindow="520" windowWidth="29380" windowHeight="20280" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -561,9 +561,6 @@
     <t>[**PROJECT 1:** Leveling in Candy Crush Saga](https://datacamp.com/projects/139)  [&lt;br&gt;**PROJECT 2:** Modeling the Volatility of US Bond Yields](https://datacamp.com/projects/738)</t>
   </si>
   <si>
-    <t>[**Project:** Trends in Maryland Crime Rates](https://datacamp.com/projects/673)</t>
-  </si>
-  <si>
     <t>DataCamp Project</t>
   </si>
   <si>
@@ -664,6 +661,9 @@
   </si>
   <si>
     <t>[DataSci 9](https://www.edx.org/course/data-science-machine-learning)</t>
+  </si>
+  <si>
+    <t>[**PROJECT:** Trends in Maryland Crime Rates](https://datacamp.com/projects/673)</t>
   </si>
 </sst>
 </file>
@@ -1035,8 +1035,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" topLeftCell="C8" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1050,30 +1050,30 @@
   <sheetData>
     <row r="1" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
+        <v>163</v>
+      </c>
+      <c r="B1" s="8" t="s">
         <v>164</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="C1" s="9" t="s">
         <v>165</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="D1" s="9" t="s">
+        <v>184</v>
+      </c>
+      <c r="E1" s="9" t="s">
         <v>166</v>
       </c>
-      <c r="D1" s="9" t="s">
-        <v>185</v>
-      </c>
-      <c r="E1" s="9" t="s">
+      <c r="F1" s="9" t="s">
         <v>167</v>
       </c>
-      <c r="F1" s="9" t="s">
-        <v>168</v>
-      </c>
       <c r="G1" s="9" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="2" spans="1:8" s="2" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A2" s="8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B2" s="8" t="s">
         <v>148</v>
@@ -1082,20 +1082,20 @@
         <v>139</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E2" s="9" t="s">
         <v>147</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="G2" s="8"/>
       <c r="H2" s="6"/>
     </row>
     <row r="3" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>149</v>
@@ -1104,19 +1104,19 @@
         <v>138</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E3" s="9" t="s">
         <v>147</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="G3" s="8"/>
     </row>
     <row r="4" spans="1:8" ht="153" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B4" s="8" t="s">
         <v>150</v>
@@ -1125,13 +1125,13 @@
         <v>140</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E4" s="9" t="s">
         <v>147</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="G4" s="9" t="s">
         <v>157</v>
@@ -1139,7 +1139,7 @@
     </row>
     <row r="5" spans="1:8" ht="153" x14ac:dyDescent="0.2">
       <c r="A5" s="8" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B5" s="8" t="s">
         <v>151</v>
@@ -1148,13 +1148,13 @@
         <v>141</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E5" s="9" t="s">
         <v>147</v>
       </c>
       <c r="F5" s="9" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="G5" s="9" t="s">
         <v>158</v>
@@ -1162,7 +1162,7 @@
     </row>
     <row r="6" spans="1:8" ht="153" x14ac:dyDescent="0.2">
       <c r="A6" s="8" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B6" s="8" t="s">
         <v>152</v>
@@ -1171,13 +1171,13 @@
         <v>142</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E6" s="9" t="s">
         <v>147</v>
       </c>
       <c r="F6" s="9" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="G6" s="9" t="s">
         <v>161</v>
@@ -1185,7 +1185,7 @@
     </row>
     <row r="7" spans="1:8" ht="102" x14ac:dyDescent="0.2">
       <c r="A7" s="8" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B7" s="8" t="s">
         <v>153</v>
@@ -1194,19 +1194,19 @@
         <v>143</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E7" s="9" t="s">
         <v>147</v>
       </c>
       <c r="F7" s="9" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="G7" s="9"/>
     </row>
     <row r="8" spans="1:8" ht="221" x14ac:dyDescent="0.2">
       <c r="A8" s="8" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B8" s="8" t="s">
         <v>154</v>
@@ -1215,13 +1215,13 @@
         <v>144</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E8" s="9" t="s">
         <v>147</v>
       </c>
       <c r="F8" s="9" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="G8" s="9" t="s">
         <v>160</v>
@@ -1229,7 +1229,7 @@
     </row>
     <row r="9" spans="1:8" ht="102" x14ac:dyDescent="0.2">
       <c r="A9" s="8" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B9" s="8" t="s">
         <v>155</v>
@@ -1238,21 +1238,21 @@
         <v>145</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E9" s="9" t="s">
         <v>147</v>
       </c>
       <c r="F9" s="9" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="G9" s="10" t="s">
-        <v>162</v>
+        <v>196</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="238" x14ac:dyDescent="0.2">
       <c r="A10" s="8" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B10" s="8" t="s">
         <v>156</v>
@@ -1261,13 +1261,13 @@
         <v>146</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E10" s="9" t="s">
         <v>147</v>
       </c>
       <c r="F10" s="9" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="G10" s="10" t="s">
         <v>159</v>

</xml_diff>

<commit_message>
Initialize the datsci page for Andy Field to check
</commit_message>
<xml_diff>
--- a/LectureSpring2019.xlsx
+++ b/LectureSpring2019.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10913"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Fatih/GitHub/dataism/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4753E83F-2E1E-B84A-BDCD-566D004F6D63}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A150330-2B56-CE40-89E5-C6D9EAB3A0F6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20" yWindow="520" windowWidth="29380" windowHeight="20280" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -630,40 +630,40 @@
     <t>**datsci Module**</t>
   </si>
   <si>
-    <t>datsci_0</t>
-  </si>
-  <si>
-    <t>datsci_1</t>
-  </si>
-  <si>
-    <t>datsci_2</t>
-  </si>
-  <si>
-    <t>datsci_3</t>
-  </si>
-  <si>
     <t xml:space="preserve">**0.** </t>
   </si>
   <si>
     <t>**1.**</t>
   </si>
   <si>
-    <t>datsci_4</t>
-  </si>
-  <si>
-    <t>datsci_5</t>
-  </si>
-  <si>
-    <t>datsci_6</t>
-  </si>
-  <si>
-    <t>datsci_7</t>
-  </si>
-  <si>
-    <t>datsci_8</t>
-  </si>
-  <si>
     <t>Available by trimester start</t>
+  </si>
+  <si>
+    <t>datsci_00</t>
+  </si>
+  <si>
+    <t>datsci_01</t>
+  </si>
+  <si>
+    <t>datsci_02</t>
+  </si>
+  <si>
+    <t>datsci_03</t>
+  </si>
+  <si>
+    <t>datsci_04</t>
+  </si>
+  <si>
+    <t>datsci_05</t>
+  </si>
+  <si>
+    <t>datsci_06</t>
+  </si>
+  <si>
+    <t>datsci_07</t>
+  </si>
+  <si>
+    <t>datsci_08</t>
   </si>
 </sst>
 </file>
@@ -1045,8 +1045,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1083,7 +1083,7 @@
     </row>
     <row r="2" spans="1:8" s="2" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A2" s="8" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="B2" s="8" t="s">
         <v>147</v>
@@ -1092,10 +1092,10 @@
         <v>139</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>196</v>
+        <v>187</v>
       </c>
       <c r="F2" s="9" t="s">
         <v>174</v>
@@ -1105,7 +1105,7 @@
     </row>
     <row r="3" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>148</v>
@@ -1114,10 +1114,10 @@
         <v>138</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>196</v>
+        <v>187</v>
       </c>
       <c r="F3" s="9" t="s">
         <v>175</v>
@@ -1135,10 +1135,10 @@
         <v>140</v>
       </c>
       <c r="D4" s="11" t="s">
+        <v>190</v>
+      </c>
+      <c r="E4" s="9" t="s">
         <v>187</v>
-      </c>
-      <c r="E4" s="9" t="s">
-        <v>196</v>
       </c>
       <c r="F4" s="9" t="s">
         <v>179</v>
@@ -1158,10 +1158,10 @@
         <v>141</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>196</v>
+        <v>187</v>
       </c>
       <c r="F5" s="9" t="s">
         <v>176</v>
@@ -1181,10 +1181,10 @@
         <v>142</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>196</v>
+        <v>187</v>
       </c>
       <c r="F6" s="9" t="s">
         <v>178</v>
@@ -1204,10 +1204,10 @@
         <v>143</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>196</v>
+        <v>187</v>
       </c>
       <c r="F7" s="9" t="s">
         <v>177</v>
@@ -1225,10 +1225,10 @@
         <v>144</v>
       </c>
       <c r="D8" s="11" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>196</v>
+        <v>187</v>
       </c>
       <c r="F8" s="9" t="s">
         <v>181</v>
@@ -1248,10 +1248,10 @@
         <v>145</v>
       </c>
       <c r="D9" s="11" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>196</v>
+        <v>187</v>
       </c>
       <c r="F9" s="9" t="s">
         <v>180</v>
@@ -1271,10 +1271,10 @@
         <v>146</v>
       </c>
       <c r="D10" s="11" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>196</v>
+        <v>187</v>
       </c>
       <c r="F10" s="9" t="s">
         <v>182</v>

</xml_diff>